<commit_message>
Compute DGF Population 1 OFF
</commit_message>
<xml_diff>
--- a/data/mapping.xlsx
+++ b/data/mapping.xlsx
@@ -430,15 +430,15 @@
     <t xml:space="preserve">Dotation de solidarité urbaine - Montant attribution spontanée DSU</t>
   </si>
   <si>
+    <t xml:space="preserve">dotation_solidarite_urbaine</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dotation de solidarité urbaine - Montant progression de la DSU</t>
   </si>
   <si>
     <t xml:space="preserve">Dotation de solidarité urbaine - Montant total réparti</t>
   </si>
   <si>
-    <t xml:space="preserve">dotation_solidarite_urbaine</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dotation nationale de péréquation - Montant part principale</t>
   </si>
   <si>
@@ -469,13 +469,13 @@
     <t xml:space="preserve">Dotation de solidarité rurale Bourg-centre - Montant de la commune éligible</t>
   </si>
   <si>
+    <t xml:space="preserve">premiere_fraction_dotation_solidarite_rurale</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dotation de solidarité rurale Bourg-centre - Montant de la garantie de sortie</t>
   </si>
   <si>
     <t xml:space="preserve">Dotation de solidarité rurale Bourg-centre - Montant global réparti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">premiere_fraction_dotation_solidarite_rurale</t>
   </si>
   <si>
     <t xml:space="preserve">Dotation de solidarité rurale Bourg-centre - Population DGF plafonnée</t>
@@ -685,8 +685,8 @@
   </sheetPr>
   <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="181" zoomScaleNormal="181" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="181" zoomScaleNormal="181" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B142" activeCellId="0" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1362,17 +1362,17 @@
       <c r="A130" s="0" t="s">
         <v>135</v>
       </c>
+      <c r="B130" s="0" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B132" s="0" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1425,17 +1425,17 @@
       <c r="A142" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="B142" s="0" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B144" s="0" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>